<commit_message>
CARGA BASE DATOS Y MODIFICACIONES EN VENTANAS
</commit_message>
<xml_diff>
--- a/Docu/Modelo_ee_Informacion.xlsx
+++ b/Docu/Modelo_ee_Informacion.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAEDE4A-6AC6-4706-B5A6-18812AD74DF9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AD4122-66D5-4FB8-99FB-0D8DA804D5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15975" windowHeight="8070" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portada" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,15 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1070,7 +1079,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyBorder="1"/>
@@ -1083,7 +1092,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2784,7 +2792,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A2:E59" totalsRowShown="0" tableBorderDxfId="3">
   <autoFilter ref="A2:E59" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState ref="A3:E59">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E59">
     <sortCondition descending="1" ref="D2:D59"/>
   </sortState>
   <tableColumns count="5">
@@ -2801,7 +2809,7 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla1" displayName="Tabla1" ref="A2:G11" totalsRowShown="0" tableBorderDxfId="2">
   <autoFilter ref="A2:G11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A3:G10">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G10">
     <sortCondition ref="A2:A10"/>
   </sortState>
   <tableColumns count="7">
@@ -3179,15 +3187,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -3195,7 +3203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -3203,7 +3211,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
@@ -3211,7 +3219,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
@@ -3219,16 +3227,16 @@
         <v>44862</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="8">
         <f ca="1">NOW()</f>
-        <v>44983.911836342595</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>44989.770842361111</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3236,7 +3244,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
@@ -3244,7 +3252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
@@ -3252,7 +3260,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
@@ -3280,25 +3288,25 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:5" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3315,7 +3323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4</v>
       </c>
@@ -3329,7 +3337,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6</v>
       </c>
@@ -3343,7 +3351,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7</v>
       </c>
@@ -3357,7 +3365,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9</v>
       </c>
@@ -3371,7 +3379,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10</v>
       </c>
@@ -3385,7 +3393,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>12</v>
       </c>
@@ -3399,7 +3407,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>13</v>
       </c>
@@ -3413,7 +3421,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>17</v>
       </c>
@@ -3427,7 +3435,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>21</v>
       </c>
@@ -3441,7 +3449,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>22</v>
       </c>
@@ -3455,7 +3463,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>23</v>
       </c>
@@ -3469,7 +3477,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>24</v>
       </c>
@@ -3483,7 +3491,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>27</v>
       </c>
@@ -3497,7 +3505,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>28</v>
       </c>
@@ -3511,7 +3519,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>29</v>
       </c>
@@ -3525,7 +3533,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>33</v>
       </c>
@@ -3539,7 +3547,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>34</v>
       </c>
@@ -3553,7 +3561,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>37</v>
       </c>
@@ -3567,7 +3575,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>39</v>
       </c>
@@ -3581,7 +3589,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>40</v>
       </c>
@@ -3595,7 +3603,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>42</v>
       </c>
@@ -3609,7 +3617,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>43</v>
       </c>
@@ -3623,7 +3631,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>44</v>
       </c>
@@ -3637,7 +3645,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>45</v>
       </c>
@@ -3651,7 +3659,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>46</v>
       </c>
@@ -3665,7 +3673,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>47</v>
       </c>
@@ -3679,7 +3687,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>48</v>
       </c>
@@ -3693,7 +3701,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>50</v>
       </c>
@@ -3707,7 +3715,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>51</v>
       </c>
@@ -3721,7 +3729,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>52</v>
       </c>
@@ -3735,7 +3743,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>53</v>
       </c>
@@ -3749,7 +3757,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>54</v>
       </c>
@@ -3763,7 +3771,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>55</v>
       </c>
@@ -3777,7 +3785,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>57</v>
       </c>
@@ -3794,7 +3802,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
@@ -3808,7 +3816,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2</v>
       </c>
@@ -3822,7 +3830,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3</v>
       </c>
@@ -3836,7 +3844,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>5</v>
       </c>
@@ -3850,7 +3858,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>14</v>
       </c>
@@ -3864,7 +3872,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>15</v>
       </c>
@@ -3878,7 +3886,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>19</v>
       </c>
@@ -3892,7 +3900,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>20</v>
       </c>
@@ -3906,7 +3914,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>26</v>
       </c>
@@ -3920,7 +3928,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>31</v>
       </c>
@@ -3934,7 +3942,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>32</v>
       </c>
@@ -3948,7 +3956,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>35</v>
       </c>
@@ -3965,7 +3973,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>36</v>
       </c>
@@ -3979,7 +3987,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>38</v>
       </c>
@@ -3993,7 +4001,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>41</v>
       </c>
@@ -4007,7 +4015,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>49</v>
       </c>
@@ -4021,7 +4029,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>56</v>
       </c>
@@ -4038,7 +4046,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>8</v>
       </c>
@@ -4055,7 +4063,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>11</v>
       </c>
@@ -4072,7 +4080,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>16</v>
       </c>
@@ -4089,7 +4097,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>18</v>
       </c>
@@ -4106,7 +4114,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>25</v>
       </c>
@@ -4123,7 +4131,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>30</v>
       </c>
@@ -4159,29 +4167,29 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -4204,7 +4212,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4227,7 +4235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4250,7 +4258,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4274,7 +4282,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4297,7 +4305,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4320,7 +4328,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4343,7 +4351,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4366,7 +4374,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4389,7 +4397,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4431,23 +4439,23 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>271</v>
       </c>
@@ -4461,8 +4469,8 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>272</v>
       </c>
       <c r="B5" t="s">
@@ -4478,233 +4486,233 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6">
         <v>6</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6">
         <v>44</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6">
         <v>427</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6">
         <v>11</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6">
         <v>471</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7">
         <v>226</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7">
         <v>49</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7">
         <v>11</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7">
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8">
         <v>18</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8">
         <v>113</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8">
         <v>6</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9">
         <v>256</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9">
         <v>63</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9">
         <v>5</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9">
         <v>319</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10">
         <v>220</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10">
         <v>113</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10">
         <v>6</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10">
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11">
         <v>7</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11">
         <v>19</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11">
         <v>235</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11">
         <v>10</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11">
         <v>254</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12">
         <v>19</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12">
         <v>12</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12">
         <v>1873</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12">
         <v>224</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12">
         <v>31</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12">
         <v>2097</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13">
         <v>6</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13">
         <v>6</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13">
         <v>106</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13">
         <v>78</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13">
         <v>12</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13">
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14">
         <v>3</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14">
         <v>16</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14">
         <v>11</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14">
         <v>5</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15">
         <v>47</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15">
         <v>50</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15">
         <v>2778</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15">
         <v>1313</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15">
         <v>97</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15">
         <v>4091</v>
       </c>
     </row>
@@ -4717,40 +4725,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53:D82"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:13" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -4791,7 +4799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4820,7 +4828,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4846,7 +4854,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4872,7 +4880,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4898,7 +4906,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4924,7 +4932,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4950,7 +4958,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4976,7 +4984,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -5002,7 +5010,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -5028,7 +5036,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -5054,7 +5062,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -5080,7 +5088,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -5109,7 +5117,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -5138,7 +5146,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -5164,7 +5172,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -5190,7 +5198,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -5216,7 +5224,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -5242,7 +5250,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -5268,7 +5276,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -5297,7 +5305,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -5323,7 +5331,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -5349,7 +5357,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -5375,7 +5383,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -5404,7 +5412,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -5430,7 +5438,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -5456,7 +5464,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -5482,7 +5490,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -5508,7 +5516,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -5534,7 +5542,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -5563,7 +5571,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -5589,7 +5597,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -5615,7 +5623,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -5641,7 +5649,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -5667,7 +5675,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -5696,7 +5704,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -5722,7 +5730,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -5748,7 +5756,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -5774,7 +5782,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -5800,7 +5808,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -5826,7 +5834,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -5855,7 +5863,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -5881,7 +5889,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -5907,7 +5915,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -5933,7 +5941,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -5959,7 +5967,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -5988,7 +5996,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -6014,7 +6022,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -6040,7 +6048,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -6066,7 +6074,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -6092,7 +6100,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -6121,7 +6129,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -6150,7 +6158,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -6182,7 +6190,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -6214,7 +6222,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -6240,7 +6248,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -6266,7 +6274,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -6292,7 +6300,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -6318,7 +6326,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -6344,7 +6352,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -6370,7 +6378,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -6396,7 +6404,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -6422,7 +6430,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -6448,7 +6456,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -6474,7 +6482,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -6500,7 +6508,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -6526,7 +6534,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -6552,7 +6560,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -6578,7 +6586,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -6604,7 +6612,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -6630,7 +6638,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -6656,7 +6664,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -6682,7 +6690,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -6708,7 +6716,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -6734,7 +6742,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -6760,7 +6768,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -6786,7 +6794,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -6812,7 +6820,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -6838,7 +6846,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -6864,7 +6872,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -6890,7 +6898,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -6916,7 +6924,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -6945,7 +6953,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -6974,7 +6982,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -7000,7 +7008,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -7026,7 +7034,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
@@ -7052,7 +7060,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
@@ -7078,7 +7086,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -7104,7 +7112,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
@@ -7130,7 +7138,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
@@ -7156,7 +7164,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -7182,7 +7190,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
@@ -7208,7 +7216,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
@@ -7234,7 +7242,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
@@ -7263,7 +7271,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
@@ -7292,7 +7300,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
@@ -7321,7 +7329,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>96</v>
       </c>
@@ -7350,7 +7358,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>97</v>
       </c>
@@ -7396,21 +7404,21 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -7424,7 +7432,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -7438,7 +7446,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -7452,7 +7460,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -7466,7 +7474,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -7480,7 +7488,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7494,7 +7502,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -7508,7 +7516,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -7522,7 +7530,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -7536,7 +7544,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -7550,7 +7558,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -7564,7 +7572,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -7578,7 +7586,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -7592,7 +7600,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -7606,7 +7614,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Modificaciones generales terminadas y nuevas tablas
</commit_message>
<xml_diff>
--- a/Docu/Modelo_ee_Informacion.xlsx
+++ b/Docu/Modelo_ee_Informacion.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAEDE4A-6AC6-4706-B5A6-18812AD74DF9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E0AD5E-D81F-4279-8D05-0A1438947094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15975" windowHeight="8070" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portada" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,15 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1070,7 +1079,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyBorder="1"/>
@@ -1083,7 +1092,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2784,7 +2792,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A2:E59" totalsRowShown="0" tableBorderDxfId="3">
   <autoFilter ref="A2:E59" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState ref="A3:E59">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E59">
     <sortCondition descending="1" ref="D2:D59"/>
   </sortState>
   <tableColumns count="5">
@@ -2801,7 +2809,7 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla1" displayName="Tabla1" ref="A2:G11" totalsRowShown="0" tableBorderDxfId="2">
   <autoFilter ref="A2:G11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A3:G10">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G10">
     <sortCondition ref="A2:A10"/>
   </sortState>
   <tableColumns count="7">
@@ -3176,18 +3184,18 @@
   <dimension ref="B1:C10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -3195,7 +3203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -3203,7 +3211,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
@@ -3211,7 +3219,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
@@ -3219,16 +3227,16 @@
         <v>44862</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="8">
         <f ca="1">NOW()</f>
-        <v>44983.911836342595</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>45026.755649999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3236,7 +3244,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
@@ -3244,7 +3252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
@@ -3252,7 +3260,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
@@ -3276,29 +3284,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:5" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3315,7 +3323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4</v>
       </c>
@@ -3329,7 +3337,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6</v>
       </c>
@@ -3343,7 +3351,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7</v>
       </c>
@@ -3357,7 +3365,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9</v>
       </c>
@@ -3371,7 +3379,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10</v>
       </c>
@@ -3385,7 +3393,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>12</v>
       </c>
@@ -3399,7 +3407,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>13</v>
       </c>
@@ -3413,7 +3421,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>17</v>
       </c>
@@ -3427,7 +3435,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>21</v>
       </c>
@@ -3441,7 +3449,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>22</v>
       </c>
@@ -3455,7 +3463,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>23</v>
       </c>
@@ -3469,7 +3477,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>24</v>
       </c>
@@ -3483,7 +3491,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>27</v>
       </c>
@@ -3497,7 +3505,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>28</v>
       </c>
@@ -3511,7 +3519,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>29</v>
       </c>
@@ -3525,7 +3533,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>33</v>
       </c>
@@ -3539,7 +3547,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>34</v>
       </c>
@@ -3553,7 +3561,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>37</v>
       </c>
@@ -3567,7 +3575,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>39</v>
       </c>
@@ -3581,7 +3589,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>40</v>
       </c>
@@ -3595,7 +3603,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>42</v>
       </c>
@@ -3609,7 +3617,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>43</v>
       </c>
@@ -3623,7 +3631,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>44</v>
       </c>
@@ -3637,7 +3645,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>45</v>
       </c>
@@ -3651,7 +3659,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>46</v>
       </c>
@@ -3665,7 +3673,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>47</v>
       </c>
@@ -3679,7 +3687,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>48</v>
       </c>
@@ -3693,7 +3701,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>50</v>
       </c>
@@ -3707,7 +3715,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>51</v>
       </c>
@@ -3721,7 +3729,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>52</v>
       </c>
@@ -3735,7 +3743,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>53</v>
       </c>
@@ -3749,7 +3757,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>54</v>
       </c>
@@ -3763,7 +3771,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>55</v>
       </c>
@@ -3777,7 +3785,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>57</v>
       </c>
@@ -3794,7 +3802,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
@@ -3808,7 +3816,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2</v>
       </c>
@@ -3822,7 +3830,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3</v>
       </c>
@@ -3836,7 +3844,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>5</v>
       </c>
@@ -3850,7 +3858,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>14</v>
       </c>
@@ -3864,7 +3872,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>15</v>
       </c>
@@ -3878,7 +3886,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>19</v>
       </c>
@@ -3892,7 +3900,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>20</v>
       </c>
@@ -3906,7 +3914,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>26</v>
       </c>
@@ -3920,7 +3928,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>31</v>
       </c>
@@ -3934,7 +3942,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>32</v>
       </c>
@@ -3948,7 +3956,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>35</v>
       </c>
@@ -3965,7 +3973,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>36</v>
       </c>
@@ -3979,7 +3987,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>38</v>
       </c>
@@ -3993,7 +4001,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>41</v>
       </c>
@@ -4007,7 +4015,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>49</v>
       </c>
@@ -4021,7 +4029,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>56</v>
       </c>
@@ -4038,7 +4046,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>8</v>
       </c>
@@ -4055,7 +4063,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>11</v>
       </c>
@@ -4072,7 +4080,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>16</v>
       </c>
@@ -4089,7 +4097,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>18</v>
       </c>
@@ -4106,7 +4114,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>25</v>
       </c>
@@ -4123,7 +4131,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>30</v>
       </c>
@@ -4159,29 +4167,29 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -4204,7 +4212,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4227,7 +4235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4250,7 +4258,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4274,7 +4282,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4297,7 +4305,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4320,7 +4328,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4343,7 +4351,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4366,7 +4374,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4389,7 +4397,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4431,23 +4439,23 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>271</v>
       </c>
@@ -4461,8 +4469,8 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>272</v>
       </c>
       <c r="B5" t="s">
@@ -4478,233 +4486,233 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6">
         <v>6</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6">
         <v>44</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6">
         <v>427</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6">
         <v>11</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6">
         <v>471</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7">
         <v>226</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7">
         <v>49</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7">
         <v>11</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7">
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8">
         <v>18</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8">
         <v>113</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8">
         <v>6</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9">
         <v>256</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9">
         <v>63</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9">
         <v>5</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9">
         <v>319</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10">
         <v>220</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10">
         <v>113</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10">
         <v>6</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10">
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11">
         <v>7</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11">
         <v>19</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11">
         <v>235</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11">
         <v>10</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11">
         <v>254</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12">
         <v>19</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12">
         <v>12</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12">
         <v>1873</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12">
         <v>224</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12">
         <v>31</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12">
         <v>2097</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13">
         <v>6</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13">
         <v>6</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13">
         <v>106</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13">
         <v>78</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13">
         <v>12</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13">
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14">
         <v>3</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14">
         <v>16</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14">
         <v>11</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14">
         <v>5</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15">
         <v>47</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15">
         <v>50</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15">
         <v>2778</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15">
         <v>1313</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15">
         <v>97</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15">
         <v>4091</v>
       </c>
     </row>
@@ -4717,40 +4725,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53:D82"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:13" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -4791,7 +4799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4820,7 +4828,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4846,7 +4854,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4872,7 +4880,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4898,7 +4906,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4924,7 +4932,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4950,7 +4958,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4976,7 +4984,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -5002,7 +5010,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -5028,7 +5036,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -5054,7 +5062,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -5080,7 +5088,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -5109,7 +5117,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -5138,7 +5146,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -5164,7 +5172,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -5190,7 +5198,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -5216,7 +5224,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -5242,7 +5250,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -5268,7 +5276,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -5297,7 +5305,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -5323,7 +5331,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -5349,7 +5357,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -5375,7 +5383,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -5404,7 +5412,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -5430,7 +5438,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -5456,7 +5464,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -5482,7 +5490,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -5508,7 +5516,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -5534,7 +5542,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -5563,7 +5571,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -5589,7 +5597,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -5615,7 +5623,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -5641,7 +5649,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -5667,7 +5675,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -5696,7 +5704,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -5722,7 +5730,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -5748,7 +5756,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -5774,7 +5782,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -5800,7 +5808,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -5826,7 +5834,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -5855,7 +5863,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -5881,7 +5889,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -5907,7 +5915,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -5933,7 +5941,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -5959,7 +5967,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -5988,7 +5996,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -6014,7 +6022,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -6040,7 +6048,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -6066,7 +6074,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -6092,7 +6100,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -6121,7 +6129,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -6150,7 +6158,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -6182,7 +6190,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -6214,7 +6222,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -6240,7 +6248,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -6266,7 +6274,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -6292,7 +6300,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -6318,7 +6326,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -6344,7 +6352,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -6370,7 +6378,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -6396,7 +6404,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -6422,7 +6430,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -6448,7 +6456,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -6474,7 +6482,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -6500,7 +6508,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -6526,7 +6534,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -6552,7 +6560,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -6578,7 +6586,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -6604,7 +6612,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -6630,7 +6638,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -6656,7 +6664,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -6682,7 +6690,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -6708,7 +6716,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -6734,7 +6742,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -6760,7 +6768,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -6786,7 +6794,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -6812,7 +6820,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -6838,7 +6846,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -6864,7 +6872,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -6890,7 +6898,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -6916,7 +6924,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -6945,7 +6953,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -6974,7 +6982,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -7000,7 +7008,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -7026,7 +7034,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
@@ -7052,7 +7060,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
@@ -7078,7 +7086,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -7104,7 +7112,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
@@ -7130,7 +7138,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
@@ -7156,7 +7164,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -7182,7 +7190,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
@@ -7208,7 +7216,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
@@ -7234,7 +7242,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
@@ -7263,7 +7271,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
@@ -7292,7 +7300,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
@@ -7321,7 +7329,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>96</v>
       </c>
@@ -7350,7 +7358,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>97</v>
       </c>
@@ -7392,25 +7400,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -7424,7 +7432,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -7438,7 +7446,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -7452,7 +7460,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -7466,7 +7474,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -7480,7 +7488,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7494,7 +7502,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -7508,7 +7516,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -7522,7 +7530,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -7536,7 +7544,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -7550,7 +7558,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -7564,7 +7572,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -7578,7 +7586,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -7592,7 +7600,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -7606,7 +7614,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>

</xml_diff>